<commit_message>
adding apache poi optimised code
</commit_message>
<xml_diff>
--- a/Data/Book1.xlsx
+++ b/Data/Book1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="11">
   <si>
     <t>TestCase</t>
   </si>
@@ -56,10 +56,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -93,6 +93,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -101,10 +108,34 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -125,10 +156,46 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -141,74 +208,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -223,37 +223,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -265,19 +367,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,121 +403,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -417,11 +417,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -445,48 +460,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -514,153 +488,179 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1076,7 +1076,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="E2" sqref="A1:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88495575221239" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="3"/>
@@ -1105,8 +1105,8 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
+      <c r="D2">
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>